<commit_message>
Rw Updates - CleanUP Drive
Rw Updates - CleanUP Drive

InCapacity - [0] , NodeW - [-3] , BirdW - [6] , FuelW - [33]

Host - [9 + 3]
</commit_message>
<xml_diff>
--- a/System_2.2.0.xlsx
+++ b/System_2.2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A358D2-CF2A-4FF2-B6DC-83766392CE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B232C8B-D143-4524-9A89-1665802FBA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="622">
   <si>
     <t>Zone</t>
   </si>
@@ -1905,15 +1905,6 @@
   </si>
   <si>
     <t>Rbangla</t>
-  </si>
-  <si>
-    <t>2 F INCapacity</t>
-  </si>
-  <si>
-    <t>15F</t>
-  </si>
-  <si>
-    <t>3M 3F</t>
   </si>
 </sst>
 </file>
@@ -4988,6 +4979,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5036,6 +5030,159 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5054,12 +5201,6 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5114,169 +5255,61 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5318,43 +5351,70 @@
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5378,112 +5438,25 @@
     <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5561,29 +5534,47 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5880,8 +5871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5937,10 +5928,10 @@
       <c r="I2" s="391" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="601" t="s">
+      <c r="J2" s="602" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="602"/>
+      <c r="K2" s="603"/>
       <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
@@ -5950,14 +5941,14 @@
       <c r="N2" s="349" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="603" t="s">
+      <c r="O2" s="604" t="s">
         <v>375</v>
       </c>
-      <c r="P2" s="604"/>
-      <c r="Q2" s="605"/>
-      <c r="R2" s="605"/>
-      <c r="S2" s="605"/>
-      <c r="T2" s="606" t="s">
+      <c r="P2" s="605"/>
+      <c r="Q2" s="606"/>
+      <c r="R2" s="606"/>
+      <c r="S2" s="606"/>
+      <c r="T2" s="607" t="s">
         <v>376</v>
       </c>
       <c r="V2" s="21" t="s">
@@ -5971,7 +5962,7 @@
       <c r="C3" s="165" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="598"/>
+      <c r="D3" s="599"/>
       <c r="E3" s="337"/>
       <c r="F3" s="265" t="s">
         <v>68</v>
@@ -6000,7 +5991,7 @@
       <c r="S3" s="24">
         <v>1</v>
       </c>
-      <c r="T3" s="607"/>
+      <c r="T3" s="608"/>
       <c r="U3" s="19" t="s">
         <v>566</v>
       </c>
@@ -6016,7 +6007,7 @@
       <c r="C4" s="165" t="s">
         <v>354</v>
       </c>
-      <c r="D4" s="599"/>
+      <c r="D4" s="600"/>
       <c r="E4" s="61"/>
       <c r="F4" s="359" t="s">
         <v>42</v>
@@ -6033,7 +6024,7 @@
       </c>
       <c r="O4" s="6"/>
       <c r="P4" s="313"/>
-      <c r="T4" s="607"/>
+      <c r="T4" s="608"/>
     </row>
     <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -6042,7 +6033,7 @@
       <c r="C5" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="600"/>
+      <c r="D5" s="601"/>
       <c r="F5" s="363" t="s">
         <v>42</v>
       </c>
@@ -6059,7 +6050,7 @@
         <v>503</v>
       </c>
       <c r="P5" s="313"/>
-      <c r="T5" s="607"/>
+      <c r="T5" s="608"/>
       <c r="U5" s="204" t="s">
         <v>225</v>
       </c>
@@ -6096,7 +6087,7 @@
       <c r="P6" s="313"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="6"/>
-      <c r="T6" s="607"/>
+      <c r="T6" s="608"/>
     </row>
     <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="209" t="s">
@@ -6134,7 +6125,7 @@
       <c r="S7" s="24">
         <v>1</v>
       </c>
-      <c r="T7" s="607"/>
+      <c r="T7" s="608"/>
     </row>
     <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -6163,7 +6154,7 @@
       <c r="P8" s="313"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="6"/>
-      <c r="T8" s="607"/>
+      <c r="T8" s="608"/>
     </row>
     <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -6202,7 +6193,7 @@
       <c r="S9" s="24">
         <v>1</v>
       </c>
-      <c r="T9" s="607"/>
+      <c r="T9" s="608"/>
     </row>
     <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -6232,7 +6223,7 @@
         <v>503</v>
       </c>
       <c r="P10" s="313"/>
-      <c r="T10" s="607"/>
+      <c r="T10" s="608"/>
     </row>
     <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -6272,7 +6263,7 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="T11" s="607"/>
+      <c r="T11" s="608"/>
       <c r="U11" s="204" t="s">
         <v>224</v>
       </c>
@@ -6305,7 +6296,7 @@
       <c r="P12" s="313"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="142"/>
-      <c r="T12" s="607"/>
+      <c r="T12" s="608"/>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="256" t="s">
@@ -6335,7 +6326,7 @@
       </c>
       <c r="P13" s="313"/>
       <c r="R13" s="142"/>
-      <c r="T13" s="607"/>
+      <c r="T13" s="608"/>
       <c r="U13" s="2" t="s">
         <v>587</v>
       </c>
@@ -6345,7 +6336,7 @@
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P14" s="313"/>
-      <c r="T14" s="607"/>
+      <c r="T14" s="608"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -6371,8 +6362,8 @@
       <c r="L15" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="595"/>
-      <c r="N15" s="598" t="s">
+      <c r="M15" s="596"/>
+      <c r="N15" s="599" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="474" t="s">
@@ -6385,7 +6376,7 @@
       <c r="S15" s="24">
         <v>1</v>
       </c>
-      <c r="T15" s="607"/>
+      <c r="T15" s="608"/>
     </row>
     <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="462" t="s">
@@ -6411,8 +6402,8 @@
       <c r="L16" s="194" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="596"/>
-      <c r="N16" s="599"/>
+      <c r="M16" s="597"/>
+      <c r="N16" s="600"/>
       <c r="P16" s="313">
         <v>1</v>
       </c>
@@ -6425,7 +6416,7 @@
       <c r="S16" s="112">
         <v>1</v>
       </c>
-      <c r="T16" s="607"/>
+      <c r="T16" s="608"/>
     </row>
     <row r="17" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
@@ -6449,8 +6440,8 @@
       <c r="L17" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="597"/>
-      <c r="N17" s="600"/>
+      <c r="M17" s="598"/>
+      <c r="N17" s="601"/>
       <c r="O17" s="474" t="s">
         <v>44</v>
       </c>
@@ -6463,11 +6454,11 @@
       <c r="S17" s="24">
         <v>1</v>
       </c>
-      <c r="T17" s="607"/>
+      <c r="T17" s="608"/>
     </row>
     <row r="18" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P18" s="313"/>
-      <c r="T18" s="607"/>
+      <c r="T18" s="608"/>
     </row>
     <row r="19" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
@@ -6491,12 +6482,12 @@
       <c r="L19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="595"/>
+      <c r="M19" s="596"/>
       <c r="N19" s="390" t="s">
         <v>503</v>
       </c>
       <c r="P19" s="313"/>
-      <c r="T19" s="607"/>
+      <c r="T19" s="608"/>
     </row>
     <row r="20" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="241" t="s">
@@ -6522,7 +6513,7 @@
       <c r="L20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="596"/>
+      <c r="M20" s="597"/>
       <c r="N20" s="383" t="s">
         <v>26</v>
       </c>
@@ -6533,7 +6524,7 @@
       <c r="S20" s="24">
         <v>1</v>
       </c>
-      <c r="T20" s="607"/>
+      <c r="T20" s="608"/>
     </row>
     <row r="21" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="241" t="s">
@@ -6559,7 +6550,7 @@
       <c r="L21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="596"/>
+      <c r="M21" s="597"/>
       <c r="N21" s="383" t="s">
         <v>18</v>
       </c>
@@ -6570,11 +6561,11 @@
       <c r="S21" s="24">
         <v>1</v>
       </c>
-      <c r="T21" s="607"/>
-      <c r="U21" s="593" t="s">
+      <c r="T21" s="608"/>
+      <c r="U21" s="594" t="s">
         <v>223</v>
       </c>
-      <c r="V21" s="594"/>
+      <c r="V21" s="595"/>
     </row>
     <row r="22" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="270" t="s">
@@ -6598,15 +6589,13 @@
       <c r="L22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="596"/>
+      <c r="M22" s="597"/>
       <c r="N22" s="372" t="s">
         <v>26</v>
       </c>
       <c r="P22" s="313"/>
-      <c r="T22" s="607"/>
-      <c r="X22" s="19" t="s">
-        <v>622</v>
-      </c>
+      <c r="T22" s="608"/>
+      <c r="X22" s="19"/>
     </row>
     <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
@@ -6630,12 +6619,12 @@
       <c r="L23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="596"/>
+      <c r="M23" s="597"/>
       <c r="N23" s="61" t="s">
         <v>504</v>
       </c>
       <c r="P23" s="313"/>
-      <c r="T23" s="607"/>
+      <c r="T23" s="608"/>
       <c r="U23" s="2" t="s">
         <v>620</v>
       </c>
@@ -6668,7 +6657,7 @@
       <c r="L24" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="596"/>
+      <c r="M24" s="597"/>
       <c r="N24" s="61" t="s">
         <v>26</v>
       </c>
@@ -6677,7 +6666,7 @@
       </c>
       <c r="P24" s="513"/>
       <c r="S24" s="80"/>
-      <c r="T24" s="607"/>
+      <c r="T24" s="608"/>
       <c r="X24" s="19"/>
     </row>
     <row r="25" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6704,7 +6693,7 @@
       <c r="L25" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="596"/>
+      <c r="M25" s="597"/>
       <c r="N25" s="61" t="s">
         <v>26</v>
       </c>
@@ -6720,10 +6709,8 @@
       <c r="S25" s="21">
         <v>1</v>
       </c>
-      <c r="T25" s="607"/>
-      <c r="V25" s="24" t="s">
-        <v>624</v>
-      </c>
+      <c r="T25" s="608"/>
+      <c r="V25" s="24"/>
     </row>
     <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
@@ -6747,15 +6734,13 @@
       <c r="L26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="596"/>
+      <c r="M26" s="597"/>
       <c r="N26" s="61" t="s">
         <v>505</v>
       </c>
       <c r="P26" s="313"/>
-      <c r="T26" s="607"/>
-      <c r="V26" s="24" t="s">
-        <v>623</v>
-      </c>
+      <c r="T26" s="608"/>
+      <c r="V26" s="24"/>
     </row>
     <row r="27" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="256" t="s">
@@ -6777,7 +6762,7 @@
       <c r="J27" s="387"/>
       <c r="K27" s="388"/>
       <c r="L27" s="389"/>
-      <c r="M27" s="596"/>
+      <c r="M27" s="597"/>
       <c r="N27" s="61"/>
       <c r="P27" s="313"/>
       <c r="R27" s="34" t="s">
@@ -6786,7 +6771,7 @@
       <c r="S27" s="24">
         <v>1</v>
       </c>
-      <c r="T27" s="607"/>
+      <c r="T27" s="608"/>
       <c r="W27" s="2" t="s">
         <v>580</v>
       </c>
@@ -6815,7 +6800,7 @@
       <c r="L28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M28" s="597"/>
+      <c r="M28" s="598"/>
       <c r="N28" s="61" t="s">
         <v>505</v>
       </c>
@@ -6831,7 +6816,7 @@
       <c r="S28" s="21">
         <v>1</v>
       </c>
-      <c r="T28" s="608"/>
+      <c r="T28" s="609"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6919,7 +6904,7 @@
       <c r="H1" s="97" t="s">
         <v>343</v>
       </c>
-      <c r="I1" s="659" t="s">
+      <c r="I1" s="614" t="s">
         <v>369</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -6955,7 +6940,7 @@
       <c r="X1" s="430" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="653" t="s">
+      <c r="Y1" s="658" t="s">
         <v>529</v>
       </c>
       <c r="Z1" s="406">
@@ -6980,7 +6965,7 @@
         <v>498</v>
       </c>
       <c r="AM1" s="402"/>
-      <c r="AN1" s="635"/>
+      <c r="AN1" s="641"/>
       <c r="AO1" s="338" t="s">
         <v>469</v>
       </c>
@@ -6989,23 +6974,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="617">
+      <c r="A2" s="667">
         <f ca="1">TODAY()</f>
         <v>45286</v>
       </c>
-      <c r="B2" s="619" t="s">
+      <c r="B2" s="669" t="s">
         <v>370</v>
       </c>
-      <c r="C2" s="615" t="s">
+      <c r="C2" s="646" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="621" t="s">
+      <c r="D2" s="671" t="s">
         <v>355</v>
       </c>
-      <c r="E2" s="669" t="s">
+      <c r="E2" s="610" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="640" t="s">
+      <c r="F2" s="620" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="393" t="s">
@@ -7014,31 +6999,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="660"/>
+      <c r="I2" s="615"/>
       <c r="J2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="671" t="s">
+      <c r="K2" s="612" t="s">
         <v>342</v>
       </c>
-      <c r="L2" s="672"/>
-      <c r="M2" s="640" t="s">
+      <c r="L2" s="613"/>
+      <c r="M2" s="620" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="644" t="s">
+      <c r="O2" s="650" t="s">
         <v>102</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="615" t="s">
+      <c r="Q2" s="646" t="s">
         <v>143</v>
       </c>
-      <c r="R2" s="598"/>
-      <c r="S2" s="657" t="s">
+      <c r="R2" s="599"/>
+      <c r="S2" s="635" t="s">
         <v>148</v>
       </c>
       <c r="T2" s="89"/>
@@ -7048,7 +7033,7 @@
       <c r="X2" s="431" t="s">
         <v>156</v>
       </c>
-      <c r="Y2" s="654"/>
+      <c r="Y2" s="659"/>
       <c r="Z2" s="407">
         <v>1</v>
       </c>
@@ -7071,15 +7056,15 @@
         <v>463</v>
       </c>
       <c r="AM2" s="428"/>
-      <c r="AN2" s="636"/>
+      <c r="AN2" s="642"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="618"/>
-      <c r="B3" s="620"/>
-      <c r="C3" s="616"/>
-      <c r="D3" s="622"/>
-      <c r="E3" s="670"/>
-      <c r="F3" s="641"/>
+      <c r="A3" s="668"/>
+      <c r="B3" s="670"/>
+      <c r="C3" s="647"/>
+      <c r="D3" s="672"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="621"/>
       <c r="G3" s="394" t="s">
         <v>28</v>
       </c>
@@ -7098,17 +7083,17 @@
       <c r="L3" s="201" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="641"/>
+      <c r="M3" s="621"/>
       <c r="N3" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="645"/>
+      <c r="O3" s="651"/>
       <c r="P3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="616"/>
-      <c r="R3" s="600"/>
-      <c r="S3" s="658"/>
+      <c r="Q3" s="647"/>
+      <c r="R3" s="601"/>
+      <c r="S3" s="637"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7116,7 +7101,7 @@
       <c r="X3" s="431" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="654"/>
+      <c r="Y3" s="659"/>
       <c r="Z3" s="408">
         <v>1</v>
       </c>
@@ -7125,7 +7110,7 @@
       <c r="AC3" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="AD3" s="656" t="s">
+      <c r="AD3" s="632" t="s">
         <v>455</v>
       </c>
       <c r="AE3" s="257"/>
@@ -7137,16 +7122,16 @@
       <c r="AK3" s="257"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="428"/>
-      <c r="AN3" s="636"/>
+      <c r="AN3" s="642"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="238" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="633" t="s">
+      <c r="B4" s="683" t="s">
         <v>373</v>
       </c>
-      <c r="C4" s="615" t="s">
+      <c r="C4" s="646" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="347" t="s">
@@ -7155,7 +7140,7 @@
       <c r="E4" s="378">
         <v>2</v>
       </c>
-      <c r="F4" s="641"/>
+      <c r="F4" s="621"/>
       <c r="G4" s="381" t="s">
         <v>201</v>
       </c>
@@ -7172,11 +7157,11 @@
         <v>150</v>
       </c>
       <c r="L4" s="204"/>
-      <c r="M4" s="641"/>
+      <c r="M4" s="621"/>
       <c r="N4" s="174" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="645"/>
+      <c r="O4" s="651"/>
       <c r="P4" s="2" t="s">
         <v>191</v>
       </c>
@@ -7198,12 +7183,12 @@
       <c r="X4" s="431" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="654"/>
+      <c r="Y4" s="659"/>
       <c r="Z4" s="409"/>
       <c r="AA4" s="307"/>
       <c r="AB4" s="209"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="656"/>
+      <c r="AD4" s="632"/>
       <c r="AE4" s="257"/>
       <c r="AF4" s="257"/>
       <c r="AG4" s="16"/>
@@ -7213,37 +7198,37 @@
       <c r="AK4" s="257"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="428"/>
-      <c r="AN4" s="636"/>
+      <c r="AN4" s="642"/>
       <c r="AO4" s="338" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="659" t="s">
+      <c r="A5" s="614" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="634"/>
-      <c r="C5" s="616"/>
+      <c r="B5" s="684"/>
+      <c r="C5" s="647"/>
       <c r="D5" s="61" t="s">
         <v>153</v>
       </c>
       <c r="E5" s="379">
         <v>1</v>
       </c>
-      <c r="F5" s="641"/>
-      <c r="G5" s="625" t="s">
+      <c r="F5" s="621"/>
+      <c r="G5" s="675" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="625"/>
-      <c r="I5" s="625"/>
-      <c r="J5" s="625"/>
-      <c r="K5" s="625"/>
-      <c r="L5" s="626"/>
-      <c r="M5" s="641"/>
+      <c r="H5" s="675"/>
+      <c r="I5" s="675"/>
+      <c r="J5" s="675"/>
+      <c r="K5" s="675"/>
+      <c r="L5" s="676"/>
+      <c r="M5" s="621"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="645"/>
+      <c r="O5" s="651"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7251,7 +7236,7 @@
       <c r="X5" s="431" t="s">
         <v>159</v>
       </c>
-      <c r="Y5" s="654"/>
+      <c r="Y5" s="659"/>
       <c r="Z5" s="409">
         <v>1</v>
       </c>
@@ -7274,24 +7259,24 @@
       <c r="AK5" s="257"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="428"/>
-      <c r="AN5" s="636"/>
+      <c r="AN5" s="642"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="660"/>
-      <c r="B6" s="631" t="s">
+      <c r="A6" s="615"/>
+      <c r="B6" s="681" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="661"/>
-      <c r="D6" s="662"/>
-      <c r="F6" s="641"/>
-      <c r="G6" s="627"/>
-      <c r="H6" s="627"/>
-      <c r="I6" s="627"/>
-      <c r="J6" s="627"/>
-      <c r="K6" s="627"/>
-      <c r="L6" s="628"/>
-      <c r="M6" s="641"/>
-      <c r="O6" s="645"/>
+      <c r="C6" s="629"/>
+      <c r="D6" s="630"/>
+      <c r="F6" s="621"/>
+      <c r="G6" s="677"/>
+      <c r="H6" s="677"/>
+      <c r="I6" s="677"/>
+      <c r="J6" s="677"/>
+      <c r="K6" s="677"/>
+      <c r="L6" s="678"/>
+      <c r="M6" s="621"/>
+      <c r="O6" s="651"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7301,7 +7286,7 @@
       <c r="X6" s="431" t="s">
         <v>160</v>
       </c>
-      <c r="Y6" s="654"/>
+      <c r="Y6" s="659"/>
       <c r="Z6" s="407">
         <v>1</v>
       </c>
@@ -7315,16 +7300,16 @@
       <c r="AF6" s="257"/>
       <c r="AG6" s="257"/>
       <c r="AH6" s="257"/>
-      <c r="AI6" s="650"/>
+      <c r="AI6" s="631"/>
       <c r="AJ6" s="441" t="s">
         <v>458</v>
       </c>
-      <c r="AK6" s="650" t="s">
+      <c r="AK6" s="631" t="s">
         <v>251</v>
       </c>
       <c r="AL6" s="257"/>
       <c r="AM6" s="428"/>
-      <c r="AN6" s="636"/>
+      <c r="AN6" s="642"/>
       <c r="AO6" s="338" t="s">
         <v>470</v>
       </c>
@@ -7333,7 +7318,7 @@
       <c r="A7" s="232" t="s">
         <v>572</v>
       </c>
-      <c r="B7" s="632"/>
+      <c r="B7" s="682"/>
       <c r="C7" s="202" t="s">
         <v>374</v>
       </c>
@@ -7343,7 +7328,7 @@
       <c r="E7" s="265">
         <v>3</v>
       </c>
-      <c r="F7" s="641"/>
+      <c r="F7" s="621"/>
       <c r="G7" s="395">
         <v>0</v>
       </c>
@@ -7356,14 +7341,14 @@
       <c r="J7" s="30">
         <v>0</v>
       </c>
-      <c r="K7" s="598">
+      <c r="K7" s="599">
         <v>0</v>
       </c>
       <c r="L7" s="212">
         <v>0</v>
       </c>
-      <c r="M7" s="641"/>
-      <c r="O7" s="645"/>
+      <c r="M7" s="621"/>
+      <c r="O7" s="651"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7377,7 +7362,7 @@
       <c r="X7" s="431" t="s">
         <v>161</v>
       </c>
-      <c r="Y7" s="654"/>
+      <c r="Y7" s="659"/>
       <c r="Z7" s="407">
         <v>1</v>
       </c>
@@ -7387,18 +7372,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="257"/>
       <c r="AF7" s="257"/>
-      <c r="AG7" s="656" t="s">
+      <c r="AG7" s="632" t="s">
         <v>454</v>
       </c>
       <c r="AH7" s="257"/>
-      <c r="AI7" s="650"/>
+      <c r="AI7" s="631"/>
       <c r="AJ7" s="257"/>
-      <c r="AK7" s="650"/>
+      <c r="AK7" s="631"/>
       <c r="AL7" s="80" t="s">
         <v>496</v>
       </c>
       <c r="AM7" s="428"/>
-      <c r="AN7" s="636"/>
+      <c r="AN7" s="642"/>
       <c r="AP7" s="76" t="s">
         <v>471</v>
       </c>
@@ -7415,27 +7400,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="641"/>
-      <c r="G8" s="626">
-        <v>0</v>
-      </c>
-      <c r="H8" s="623" t="s">
+      <c r="F8" s="621"/>
+      <c r="G8" s="676">
+        <v>0</v>
+      </c>
+      <c r="H8" s="673" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="598">
-        <v>0</v>
-      </c>
-      <c r="J8" s="623" t="s">
+      <c r="I8" s="599">
+        <v>0</v>
+      </c>
+      <c r="J8" s="673" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="629"/>
-      <c r="L8" s="663"/>
-      <c r="M8" s="642"/>
-      <c r="N8" s="666">
+      <c r="K8" s="679"/>
+      <c r="L8" s="633"/>
+      <c r="M8" s="648"/>
+      <c r="N8" s="638">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="645"/>
+      <c r="O8" s="651"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7445,7 +7430,7 @@
       <c r="X8" s="431" t="s">
         <v>162</v>
       </c>
-      <c r="Y8" s="654"/>
+      <c r="Y8" s="659"/>
       <c r="Z8" s="409"/>
       <c r="AA8" s="307"/>
       <c r="AB8" s="209"/>
@@ -7453,14 +7438,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="257"/>
       <c r="AF8" s="257"/>
-      <c r="AG8" s="656"/>
+      <c r="AG8" s="632"/>
       <c r="AH8" s="257"/>
-      <c r="AI8" s="650"/>
+      <c r="AI8" s="631"/>
       <c r="AJ8" s="257"/>
       <c r="AK8" s="257"/>
       <c r="AL8" s="257"/>
       <c r="AM8" s="428"/>
-      <c r="AN8" s="636"/>
+      <c r="AN8" s="642"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="232" t="s">
@@ -7475,17 +7460,17 @@
       <c r="D9" s="348" t="s">
         <v>281</v>
       </c>
-      <c r="F9" s="641"/>
-      <c r="G9" s="628"/>
-      <c r="H9" s="624"/>
-      <c r="I9" s="600"/>
-      <c r="J9" s="624"/>
-      <c r="K9" s="630"/>
-      <c r="L9" s="664"/>
-      <c r="M9" s="643"/>
-      <c r="N9" s="667"/>
-      <c r="O9" s="646"/>
-      <c r="S9" s="657" t="s">
+      <c r="F9" s="621"/>
+      <c r="G9" s="678"/>
+      <c r="H9" s="674"/>
+      <c r="I9" s="601"/>
+      <c r="J9" s="674"/>
+      <c r="K9" s="680"/>
+      <c r="L9" s="634"/>
+      <c r="M9" s="649"/>
+      <c r="N9" s="639"/>
+      <c r="O9" s="652"/>
+      <c r="S9" s="635" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="89"/>
@@ -7497,7 +7482,7 @@
       <c r="X9" s="431" t="s">
         <v>163</v>
       </c>
-      <c r="Y9" s="654"/>
+      <c r="Y9" s="659"/>
       <c r="Z9" s="410"/>
       <c r="AA9" s="307"/>
       <c r="AB9" s="209"/>
@@ -7507,16 +7492,16 @@
       </c>
       <c r="AE9" s="257"/>
       <c r="AF9" s="257"/>
-      <c r="AG9" s="656"/>
+      <c r="AG9" s="632"/>
       <c r="AH9" s="257"/>
-      <c r="AI9" s="650"/>
+      <c r="AI9" s="631"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="650" t="s">
+      <c r="AK9" s="631" t="s">
         <v>251</v>
       </c>
       <c r="AL9" s="257"/>
       <c r="AM9" s="428"/>
-      <c r="AN9" s="636"/>
+      <c r="AN9" s="642"/>
       <c r="AP9" s="2" t="s">
         <v>508</v>
       </c>
@@ -7533,20 +7518,20 @@
         <f>Boat!W8</f>
         <v>39</v>
       </c>
-      <c r="F10" s="641"/>
+      <c r="F10" s="621"/>
       <c r="N10" s="418" t="s">
         <v>396</v>
       </c>
-      <c r="O10" s="678" t="s">
+      <c r="O10" s="623" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="647" t="s">
+      <c r="P10" s="653" t="s">
         <v>400</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="665"/>
+      <c r="S10" s="636"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>176</v>
@@ -7558,7 +7543,7 @@
       <c r="X10" s="431" t="s">
         <v>164</v>
       </c>
-      <c r="Y10" s="654"/>
+      <c r="Y10" s="659"/>
       <c r="Z10" s="409">
         <v>0</v>
       </c>
@@ -7576,16 +7561,16 @@
       <c r="AF10" s="238" t="s">
         <v>311</v>
       </c>
-      <c r="AG10" s="656"/>
+      <c r="AG10" s="632"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="650"/>
+      <c r="AI10" s="631"/>
       <c r="AJ10" s="257"/>
-      <c r="AK10" s="650"/>
+      <c r="AK10" s="631"/>
       <c r="AL10" s="257"/>
       <c r="AM10" s="442" t="s">
         <v>318</v>
       </c>
-      <c r="AN10" s="636"/>
+      <c r="AN10" s="642"/>
       <c r="AO10" s="204" t="s">
         <v>94</v>
       </c>
@@ -7594,7 +7579,7 @@
       <c r="A11" s="223" t="s">
         <v>285</v>
       </c>
-      <c r="B11" s="598" t="s">
+      <c r="B11" s="599" t="s">
         <v>283</v>
       </c>
       <c r="C11" s="457" t="s">
@@ -7603,18 +7588,18 @@
       <c r="D11" s="170" t="s">
         <v>355</v>
       </c>
-      <c r="F11" s="641"/>
+      <c r="F11" s="621"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="679"/>
-      <c r="P11" s="648"/>
+      <c r="O11" s="624"/>
+      <c r="P11" s="654"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>220</v>
       </c>
-      <c r="S11" s="665"/>
+      <c r="S11" s="636"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7624,7 +7609,7 @@
       <c r="X11" s="431" t="s">
         <v>165</v>
       </c>
-      <c r="Y11" s="654"/>
+      <c r="Y11" s="659"/>
       <c r="Z11" s="409"/>
       <c r="AA11" s="307">
         <v>1</v>
@@ -7638,14 +7623,14 @@
       <c r="AF11" s="257" t="s">
         <v>476</v>
       </c>
-      <c r="AG11" s="656"/>
+      <c r="AG11" s="632"/>
       <c r="AH11" s="257"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="257"/>
       <c r="AK11" s="257"/>
       <c r="AL11" s="257"/>
       <c r="AM11" s="428"/>
-      <c r="AN11" s="636"/>
+      <c r="AN11" s="642"/>
       <c r="AP11" s="76" t="s">
         <v>484</v>
       </c>
@@ -7654,7 +7639,7 @@
       <c r="A12" s="227" t="s">
         <v>383</v>
       </c>
-      <c r="B12" s="600"/>
+      <c r="B12" s="601"/>
       <c r="C12" s="458" t="s">
         <v>384</v>
       </c>
@@ -7664,25 +7649,25 @@
       <c r="E12" s="224">
         <v>3</v>
       </c>
-      <c r="F12" s="641"/>
+      <c r="F12" s="621"/>
       <c r="G12" s="337" t="s">
         <v>400</v>
       </c>
-      <c r="H12" s="603" t="s">
+      <c r="H12" s="604" t="s">
         <v>429</v>
       </c>
-      <c r="I12" s="605"/>
-      <c r="J12" s="605"/>
-      <c r="K12" s="683"/>
+      <c r="I12" s="606"/>
+      <c r="J12" s="606"/>
+      <c r="K12" s="628"/>
       <c r="L12" s="203"/>
       <c r="M12" s="203"/>
       <c r="N12" s="203"/>
-      <c r="O12" s="679"/>
-      <c r="P12" s="648"/>
+      <c r="O12" s="624"/>
+      <c r="P12" s="654"/>
       <c r="R12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="S12" s="658"/>
+      <c r="S12" s="637"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7692,7 +7677,7 @@
       <c r="X12" s="431" t="s">
         <v>166</v>
       </c>
-      <c r="Y12" s="654"/>
+      <c r="Y12" s="659"/>
       <c r="Z12" s="407">
         <v>1</v>
       </c>
@@ -7703,16 +7688,16 @@
       <c r="AC12" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="AD12" s="668" t="s">
+      <c r="AD12" s="640" t="s">
         <v>240</v>
       </c>
       <c r="AE12" s="441" t="s">
         <v>239</v>
       </c>
-      <c r="AF12" s="656" t="s">
+      <c r="AF12" s="632" t="s">
         <v>228</v>
       </c>
-      <c r="AG12" s="656"/>
+      <c r="AG12" s="632"/>
       <c r="AH12" s="238" t="s">
         <v>259</v>
       </c>
@@ -7722,10 +7707,10 @@
       <c r="AJ12" s="257"/>
       <c r="AK12" s="257"/>
       <c r="AL12" s="257"/>
-      <c r="AM12" s="651" t="s">
+      <c r="AM12" s="656" t="s">
         <v>249</v>
       </c>
-      <c r="AN12" s="636"/>
+      <c r="AN12" s="642"/>
       <c r="AO12" s="338" t="s">
         <v>96</v>
       </c>
@@ -7737,17 +7722,17 @@
       <c r="E13" s="448">
         <v>-3</v>
       </c>
-      <c r="F13" s="641"/>
-      <c r="G13" s="605" t="s">
+      <c r="F13" s="621"/>
+      <c r="G13" s="606" t="s">
         <v>430</v>
       </c>
-      <c r="H13" s="605"/>
-      <c r="I13" s="605"/>
-      <c r="J13" s="683"/>
+      <c r="H13" s="606"/>
+      <c r="I13" s="606"/>
+      <c r="J13" s="628"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="679"/>
-      <c r="P13" s="649"/>
+      <c r="O13" s="624"/>
+      <c r="P13" s="655"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7757,7 +7742,7 @@
       <c r="X13" s="431" t="s">
         <v>167</v>
       </c>
-      <c r="Y13" s="654"/>
+      <c r="Y13" s="659"/>
       <c r="Z13" s="407">
         <v>1</v>
       </c>
@@ -7768,8 +7753,8 @@
         <v>500</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="668"/>
-      <c r="AF13" s="656"/>
+      <c r="AD13" s="640"/>
+      <c r="AF13" s="632"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="238" t="s">
         <v>308</v>
@@ -7780,8 +7765,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="257"/>
       <c r="AL13" s="257"/>
-      <c r="AM13" s="651"/>
-      <c r="AN13" s="636"/>
+      <c r="AM13" s="656"/>
+      <c r="AN13" s="642"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="450"/>
@@ -7789,18 +7774,18 @@
       <c r="C14" s="459"/>
       <c r="D14" s="452"/>
       <c r="E14" s="453"/>
-      <c r="F14" s="641"/>
-      <c r="G14" s="605" t="s">
+      <c r="F14" s="621"/>
+      <c r="G14" s="606" t="s">
         <v>429</v>
       </c>
-      <c r="H14" s="605"/>
-      <c r="I14" s="605"/>
-      <c r="J14" s="683"/>
+      <c r="H14" s="606"/>
+      <c r="I14" s="606"/>
+      <c r="J14" s="628"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="679"/>
+      <c r="O14" s="624"/>
       <c r="Q14" s="61" t="s">
         <v>533</v>
       </c>
@@ -7814,34 +7799,34 @@
       <c r="X14" s="431" t="s">
         <v>168</v>
       </c>
-      <c r="Y14" s="654"/>
+      <c r="Y14" s="659"/>
       <c r="Z14" s="407">
         <v>1</v>
       </c>
       <c r="AA14" s="307"/>
       <c r="AB14" s="209"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="668"/>
+      <c r="AD14" s="640"/>
       <c r="AE14" s="257"/>
-      <c r="AF14" s="656"/>
+      <c r="AF14" s="632"/>
       <c r="AG14" s="257"/>
       <c r="AH14" s="257"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="257"/>
       <c r="AK14" s="257"/>
       <c r="AL14" s="257"/>
-      <c r="AM14" s="651"/>
-      <c r="AN14" s="636"/>
+      <c r="AM14" s="656"/>
+      <c r="AN14" s="642"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="449" t="s">
         <v>506</v>
       </c>
-      <c r="C15" s="598" t="s">
+      <c r="C15" s="599" t="s">
         <v>373</v>
       </c>
-      <c r="F15" s="641"/>
-      <c r="O15" s="679"/>
+      <c r="F15" s="621"/>
+      <c r="O15" s="624"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7854,7 +7839,7 @@
       <c r="X15" s="431" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="654"/>
+      <c r="Y15" s="659"/>
       <c r="Z15" s="409">
         <v>1</v>
       </c>
@@ -7863,8 +7848,8 @@
       <c r="AC15" s="76" t="s">
         <v>479</v>
       </c>
-      <c r="AD15" s="668"/>
-      <c r="AF15" s="656"/>
+      <c r="AD15" s="640"/>
+      <c r="AF15" s="632"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="238" t="s">
         <v>448</v>
@@ -7877,8 +7862,8 @@
       </c>
       <c r="AK15" s="257"/>
       <c r="AL15" s="257"/>
-      <c r="AM15" s="651"/>
-      <c r="AN15" s="636"/>
+      <c r="AM15" s="656"/>
+      <c r="AN15" s="642"/>
       <c r="AP15" s="76" t="s">
         <v>73</v>
       </c>
@@ -7893,20 +7878,20 @@
       <c r="B16" s="21" t="s">
         <v>406</v>
       </c>
-      <c r="C16" s="600"/>
+      <c r="C16" s="601"/>
       <c r="D16" s="61" t="s">
         <v>493</v>
       </c>
       <c r="E16" s="224">
         <v>1</v>
       </c>
-      <c r="F16" s="641"/>
+      <c r="F16" s="621"/>
       <c r="G16" s="337" t="s">
         <v>488</v>
       </c>
       <c r="I16" s="469"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="679"/>
+      <c r="O16" s="624"/>
       <c r="R16" s="435" t="s">
         <v>184</v>
       </c>
@@ -7917,7 +7902,7 @@
       <c r="X16" s="431" t="s">
         <v>170</v>
       </c>
-      <c r="Y16" s="654"/>
+      <c r="Y16" s="659"/>
       <c r="Z16" s="407">
         <v>1</v>
       </c>
@@ -7938,18 +7923,18 @@
       <c r="AM16" s="428" t="s">
         <v>317</v>
       </c>
-      <c r="AN16" s="636"/>
+      <c r="AN16" s="642"/>
       <c r="AP16" s="76" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="641"/>
+      <c r="F17" s="621"/>
       <c r="I17" s="470"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="679"/>
+      <c r="O17" s="624"/>
       <c r="Q17" s="21" t="s">
         <v>531</v>
       </c>
@@ -7969,7 +7954,7 @@
       <c r="X17" s="431" t="s">
         <v>171</v>
       </c>
-      <c r="Y17" s="654"/>
+      <c r="Y17" s="659"/>
       <c r="Z17" s="409"/>
       <c r="AA17" s="307"/>
       <c r="AB17" s="209"/>
@@ -7994,7 +7979,7 @@
       <c r="AK17" s="257"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="428"/>
-      <c r="AN17" s="636"/>
+      <c r="AN17" s="642"/>
       <c r="AO17" s="204" t="s">
         <v>497</v>
       </c>
@@ -8018,21 +8003,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="641"/>
+      <c r="F18" s="621"/>
       <c r="G18" s="337" t="s">
         <v>528</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="679"/>
+      <c r="O18" s="624"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="673" t="s">
+      <c r="R18" s="616" t="s">
         <v>536</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="612" t="s">
+      <c r="U18" s="664" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8042,7 +8027,7 @@
       <c r="X18" s="431" t="s">
         <v>172</v>
       </c>
-      <c r="Y18" s="654"/>
+      <c r="Y18" s="659"/>
       <c r="Z18" s="409">
         <v>1</v>
       </c>
@@ -8053,38 +8038,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="257"/>
-      <c r="AF18" s="650" t="s">
+      <c r="AF18" s="631" t="s">
         <v>475</v>
       </c>
       <c r="AG18" s="257"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="652" t="s">
+      <c r="AJ18" s="657" t="s">
         <v>315</v>
       </c>
       <c r="AK18" s="257"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="428"/>
-      <c r="AN18" s="636"/>
+      <c r="AN18" s="642"/>
       <c r="AP18" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="641"/>
+      <c r="F19" s="621"/>
       <c r="I19" s="219"/>
-      <c r="O19" s="679"/>
-      <c r="R19" s="674"/>
+      <c r="O19" s="624"/>
+      <c r="R19" s="617"/>
       <c r="S19" s="30" t="s">
         <v>534</v>
       </c>
-      <c r="U19" s="613"/>
+      <c r="U19" s="665"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="431" t="s">
         <v>173</v>
       </c>
-      <c r="Y19" s="654"/>
+      <c r="Y19" s="659"/>
       <c r="Z19" s="407">
         <v>1</v>
       </c>
@@ -8093,17 +8078,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="257"/>
-      <c r="AF19" s="650"/>
+      <c r="AF19" s="631"/>
       <c r="AG19" s="257"/>
       <c r="AH19" s="257"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="652"/>
+      <c r="AJ19" s="657"/>
       <c r="AK19" s="460" t="s">
         <v>251</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="428"/>
-      <c r="AN19" s="636"/>
+      <c r="AN19" s="642"/>
       <c r="AP19" s="76" t="s">
         <v>468</v>
       </c>
@@ -8124,24 +8109,24 @@
       <c r="E20" s="437">
         <v>-1</v>
       </c>
-      <c r="F20" s="641"/>
+      <c r="F20" s="621"/>
       <c r="G20" s="337" t="s">
         <v>491</v>
       </c>
       <c r="I20" s="219"/>
-      <c r="O20" s="679"/>
-      <c r="Q20" s="681" t="s">
+      <c r="O20" s="624"/>
+      <c r="Q20" s="626" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="404" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="614"/>
+      <c r="U20" s="666"/>
       <c r="W20" s="405"/>
       <c r="X20" s="432" t="s">
         <v>174</v>
       </c>
-      <c r="Y20" s="654"/>
+      <c r="Y20" s="659"/>
       <c r="Z20" s="411">
         <v>1</v>
       </c>
@@ -8166,7 +8151,7 @@
       <c r="AM20" s="381" t="s">
         <v>249</v>
       </c>
-      <c r="AN20" s="636"/>
+      <c r="AN20" s="642"/>
       <c r="AO20" s="338" t="s">
         <v>460</v>
       </c>
@@ -8187,20 +8172,20 @@
       <c r="E21" s="265">
         <v>0</v>
       </c>
-      <c r="F21" s="641"/>
+      <c r="F21" s="621"/>
       <c r="I21" s="219"/>
-      <c r="O21" s="679"/>
-      <c r="Q21" s="682"/>
+      <c r="O21" s="624"/>
+      <c r="Q21" s="627"/>
       <c r="T21" s="422"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="609"/>
+      <c r="V21" s="661"/>
       <c r="W21" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X21" s="429" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="654"/>
+      <c r="Y21" s="659"/>
       <c r="Z21" s="445">
         <v>3</v>
       </c>
@@ -8231,15 +8216,15 @@
       <c r="AM21" s="428" t="s">
         <v>545</v>
       </c>
-      <c r="AN21" s="636"/>
+      <c r="AN21" s="642"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="641"/>
+      <c r="F22" s="621"/>
       <c r="G22" s="337" t="s">
         <v>489</v>
       </c>
       <c r="I22" s="219"/>
-      <c r="O22" s="679"/>
+      <c r="O22" s="624"/>
       <c r="R22" s="434" t="s">
         <v>44</v>
       </c>
@@ -8247,14 +8232,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="610"/>
+      <c r="V22" s="662"/>
       <c r="W22" s="426" t="s">
         <v>175</v>
       </c>
       <c r="X22" s="429" t="s">
         <v>187</v>
       </c>
-      <c r="Y22" s="654"/>
+      <c r="Y22" s="659"/>
       <c r="Z22" s="415"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="415"/>
@@ -8265,7 +8250,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="650" t="s">
+      <c r="AJ22" s="631" t="s">
         <v>472</v>
       </c>
       <c r="AK22" s="257"/>
@@ -8273,7 +8258,7 @@
         <v>478</v>
       </c>
       <c r="AM22" s="300"/>
-      <c r="AN22" s="636"/>
+      <c r="AN22" s="642"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="231" t="s">
@@ -8291,22 +8276,22 @@
       <c r="E23" s="225">
         <v>1</v>
       </c>
-      <c r="F23" s="641"/>
+      <c r="F23" s="621"/>
       <c r="I23" s="219"/>
-      <c r="O23" s="679"/>
-      <c r="Q23" s="681" t="s">
+      <c r="O23" s="624"/>
+      <c r="Q23" s="626" t="s">
         <v>144</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="420" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="610"/>
+      <c r="V23" s="662"/>
       <c r="W23" s="148"/>
       <c r="X23" s="429" t="s">
         <v>188</v>
       </c>
-      <c r="Y23" s="654"/>
+      <c r="Y23" s="659"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="415"/>
@@ -8317,13 +8302,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="650"/>
+      <c r="AJ23" s="631"/>
       <c r="AK23" s="257"/>
       <c r="AL23" s="80" t="s">
         <v>507</v>
       </c>
       <c r="AM23" s="300"/>
-      <c r="AN23" s="636"/>
+      <c r="AN23" s="642"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="440" t="s">
@@ -8341,23 +8326,23 @@
       <c r="E24" s="436">
         <v>1</v>
       </c>
-      <c r="F24" s="641"/>
+      <c r="F24" s="621"/>
       <c r="G24" s="61" t="s">
         <v>490</v>
       </c>
       <c r="I24" s="219"/>
-      <c r="O24" s="679"/>
-      <c r="Q24" s="682"/>
+      <c r="O24" s="624"/>
+      <c r="Q24" s="627"/>
       <c r="T24" s="17"/>
       <c r="U24" s="227" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="610"/>
+      <c r="V24" s="662"/>
       <c r="W24" s="148"/>
       <c r="X24" s="429" t="s">
         <v>185</v>
       </c>
-      <c r="Y24" s="654"/>
+      <c r="Y24" s="659"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="415"/>
@@ -8376,12 +8361,12 @@
         <v>463</v>
       </c>
       <c r="AM24" s="300"/>
-      <c r="AN24" s="636"/>
+      <c r="AN24" s="642"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="641"/>
+      <c r="F25" s="621"/>
       <c r="I25" s="219"/>
-      <c r="O25" s="679"/>
+      <c r="O25" s="624"/>
       <c r="P25" s="204" t="s">
         <v>280</v>
       </c>
@@ -8394,12 +8379,12 @@
       <c r="U25" s="400" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="611"/>
+      <c r="V25" s="663"/>
       <c r="W25" s="148"/>
       <c r="X25" s="429" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="654"/>
+      <c r="Y25" s="659"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="415"/>
@@ -8416,7 +8401,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="300"/>
-      <c r="AN25" s="636"/>
+      <c r="AN25" s="642"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="231" t="s">
@@ -8434,17 +8419,17 @@
       <c r="E26" s="380">
         <v>1</v>
       </c>
-      <c r="F26" s="641"/>
+      <c r="F26" s="621"/>
       <c r="G26" s="337" t="s">
         <v>487</v>
       </c>
       <c r="I26" s="219"/>
-      <c r="O26" s="679"/>
-      <c r="P26" s="638" t="s">
+      <c r="O26" s="624"/>
+      <c r="P26" s="644" t="s">
         <v>526</v>
       </c>
-      <c r="Q26" s="639"/>
-      <c r="R26" s="675" t="s">
+      <c r="Q26" s="645"/>
+      <c r="R26" s="618" t="s">
         <v>535</v>
       </c>
       <c r="T26" s="178"/>
@@ -8456,7 +8441,7 @@
       <c r="X26" s="429" t="s">
         <v>181</v>
       </c>
-      <c r="Y26" s="654"/>
+      <c r="Y26" s="659"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="415"/>
@@ -8483,7 +8468,7 @@
       <c r="AM26" s="442" t="s">
         <v>456</v>
       </c>
-      <c r="AN26" s="636"/>
+      <c r="AN26" s="642"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8495,13 +8480,13 @@
       <c r="E27" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="677"/>
+      <c r="F27" s="622"/>
       <c r="G27" s="61" t="s">
         <v>544</v>
       </c>
       <c r="I27" s="220"/>
-      <c r="O27" s="680"/>
-      <c r="R27" s="676"/>
+      <c r="O27" s="625"/>
+      <c r="R27" s="619"/>
       <c r="S27" s="421" t="s">
         <v>54</v>
       </c>
@@ -8514,7 +8499,7 @@
       <c r="X27" s="429" t="s">
         <v>530</v>
       </c>
-      <c r="Y27" s="655"/>
+      <c r="Y27" s="660"/>
       <c r="Z27" s="161"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="416"/>
@@ -8531,32 +8516,26 @@
       <c r="AM27" s="381" t="s">
         <v>319</v>
       </c>
-      <c r="AN27" s="637"/>
+      <c r="AN27" s="643"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -8573,22 +8552,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8622,15 +8607,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="603" t="s">
+      <c r="B1" s="604" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="683"/>
+      <c r="C1" s="628"/>
       <c r="D1" s="204"/>
-      <c r="J1" s="603" t="s">
+      <c r="J1" s="604" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="683"/>
+      <c r="K1" s="628"/>
       <c r="L1" s="195" t="s">
         <v>330</v>
       </c>
@@ -8668,13 +8653,13 @@
         <v>34</v>
       </c>
       <c r="L2" s="196"/>
-      <c r="M2" s="684"/>
+      <c r="M2" s="685"/>
       <c r="N2" s="153">
         <v>2</v>
       </c>
       <c r="O2" s="154"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="687" t="s">
+      <c r="Q2" s="688" t="s">
         <v>44</v>
       </c>
       <c r="R2" s="19">
@@ -8697,13 +8682,13 @@
       <c r="K3" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="M3" s="685"/>
+      <c r="M3" s="686"/>
       <c r="N3" s="17">
         <v>1</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="688"/>
+      <c r="Q3" s="689"/>
       <c r="R3" s="219"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8722,13 +8707,13 @@
       <c r="K4" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="M4" s="685"/>
+      <c r="M4" s="686"/>
       <c r="N4" s="17"/>
       <c r="O4" s="15">
         <v>1</v>
       </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="688"/>
+      <c r="Q4" s="689"/>
       <c r="R4" s="219"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8748,13 +8733,13 @@
         <v>13</v>
       </c>
       <c r="L5" s="196"/>
-      <c r="M5" s="685"/>
+      <c r="M5" s="686"/>
       <c r="N5" s="17">
         <v>1</v>
       </c>
       <c r="O5" s="15"/>
       <c r="P5" s="10"/>
-      <c r="Q5" s="688"/>
+      <c r="Q5" s="689"/>
       <c r="R5" s="19">
         <v>-1</v>
       </c>
@@ -8775,13 +8760,13 @@
       <c r="K6" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="M6" s="685"/>
+      <c r="M6" s="686"/>
       <c r="N6" s="17">
         <v>1</v>
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="688"/>
+      <c r="Q6" s="689"/>
       <c r="R6" s="219"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8801,13 +8786,13 @@
         <v>327</v>
       </c>
       <c r="L7" s="198"/>
-      <c r="M7" s="685"/>
+      <c r="M7" s="686"/>
       <c r="N7" s="17">
         <v>1</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="688"/>
+      <c r="Q7" s="689"/>
       <c r="R7" s="19">
         <v>-1</v>
       </c>
@@ -8828,13 +8813,13 @@
       <c r="K8" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="M8" s="685"/>
+      <c r="M8" s="686"/>
       <c r="N8" s="17">
         <v>1</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="688"/>
+      <c r="Q8" s="689"/>
       <c r="R8" s="219"/>
     </row>
     <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8854,13 +8839,13 @@
         <v>329</v>
       </c>
       <c r="L9" s="181"/>
-      <c r="M9" s="686"/>
+      <c r="M9" s="687"/>
       <c r="N9" s="161"/>
       <c r="O9" s="18"/>
       <c r="P9" s="13">
         <v>1</v>
       </c>
-      <c r="Q9" s="689"/>
+      <c r="Q9" s="690"/>
       <c r="R9" s="220"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -8965,7 +8950,7 @@
   <dimension ref="A1:AL31"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AG16" sqref="AG16"/>
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9033,7 +9018,7 @@
       <c r="P1" s="398" t="s">
         <v>397</v>
       </c>
-      <c r="Q1" s="714" t="s">
+      <c r="Q1" s="702" t="s">
         <v>180</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9057,7 +9042,7 @@
       <c r="AA1" s="517" t="s">
         <v>437</v>
       </c>
-      <c r="AB1" s="708" t="s">
+      <c r="AB1" s="696" t="s">
         <v>594</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9079,32 +9064,32 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="693">
+      <c r="A2" s="707">
         <f ca="1">TODAY()</f>
         <v>45286</v>
       </c>
-      <c r="B2" s="695" t="s">
+      <c r="B2" s="709" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="615" t="s">
+      <c r="C2" s="646" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="697" t="s">
+      <c r="D2" s="711" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="699" t="s">
+      <c r="E2" s="713" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="191" t="s">
         <v>218</v>
       </c>
-      <c r="G2" s="659" t="s">
+      <c r="G2" s="614" t="s">
         <v>372</v>
       </c>
       <c r="H2" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I2" s="705" t="s">
+      <c r="I2" s="693" t="s">
         <v>102</v>
       </c>
       <c r="J2" s="396" t="s">
@@ -9128,14 +9113,14 @@
       <c r="P2" s="399">
         <v>40</v>
       </c>
-      <c r="Q2" s="715"/>
+      <c r="Q2" s="703"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S20</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T2" s="172">
         <f>SUM(T4:T16)</f>
@@ -9153,31 +9138,27 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="709"/>
+      <c r="AB2" s="697"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="AI2" s="469">
-        <v>1</v>
-      </c>
+      <c r="AI2" s="469"/>
       <c r="AJ2" s="553"/>
       <c r="AK2" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="AL2" s="469">
-        <v>1</v>
-      </c>
+      <c r="AL2" s="469"/>
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="694"/>
-      <c r="B3" s="696"/>
-      <c r="C3" s="616"/>
-      <c r="D3" s="698"/>
-      <c r="E3" s="700"/>
-      <c r="G3" s="660"/>
+      <c r="A3" s="708"/>
+      <c r="B3" s="710"/>
+      <c r="C3" s="647"/>
+      <c r="D3" s="712"/>
+      <c r="E3" s="714"/>
+      <c r="G3" s="615"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="706"/>
+      <c r="I3" s="694"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9186,13 +9167,13 @@
       </c>
       <c r="Q3" s="471">
         <f>SUM(X23:X31)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="470"/>
       <c r="W3" s="6"/>
       <c r="X3" s="470"/>
-      <c r="AB3" s="709"/>
+      <c r="AB3" s="697"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>589</v>
@@ -9205,26 +9186,22 @@
       <c r="AH3" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="AI3" s="470">
-        <v>1</v>
-      </c>
+      <c r="AI3" s="470"/>
       <c r="AJ3" s="553"/>
       <c r="AK3" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AL3" s="24">
-        <v>1</v>
-      </c>
+      <c r="AL3" s="24"/>
     </row>
     <row r="4" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="236" t="s">
         <v>380</v>
       </c>
       <c r="B4" s="243"/>
-      <c r="C4" s="701" t="s">
+      <c r="C4" s="715" t="s">
         <v>177</v>
       </c>
-      <c r="I4" s="706"/>
+      <c r="I4" s="694"/>
       <c r="R4" s="471" t="s">
         <v>589</v>
       </c>
@@ -9236,7 +9213,7 @@
       <c r="V4" s="470"/>
       <c r="W4" s="6"/>
       <c r="X4" s="470"/>
-      <c r="AB4" s="709"/>
+      <c r="AB4" s="697"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9249,16 +9226,12 @@
       <c r="AH4" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AI4" s="470">
-        <v>1</v>
-      </c>
+      <c r="AI4" s="470"/>
       <c r="AJ4" s="553"/>
       <c r="AK4" s="6" t="s">
         <v>611</v>
       </c>
-      <c r="AL4" s="24">
-        <v>1</v>
-      </c>
+      <c r="AL4" s="24"/>
     </row>
     <row r="5" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="221" t="s">
@@ -9267,7 +9240,7 @@
       <c r="B5" s="100" t="s">
         <v>357</v>
       </c>
-      <c r="C5" s="702"/>
+      <c r="C5" s="716"/>
       <c r="D5" s="222" t="s">
         <v>102</v>
       </c>
@@ -9277,13 +9250,13 @@
       <c r="F5" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="G5" s="598" t="s">
+      <c r="G5" s="599" t="s">
         <v>271</v>
       </c>
       <c r="H5" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I5" s="706"/>
+      <c r="I5" s="694"/>
       <c r="J5" s="397" t="s">
         <v>268</v>
       </c>
@@ -9310,7 +9283,7 @@
       <c r="V5" s="468"/>
       <c r="W5" s="6"/>
       <c r="X5" s="468"/>
-      <c r="AB5" s="709"/>
+      <c r="AB5" s="697"/>
       <c r="AC5" s="2" t="s">
         <v>592</v>
       </c>
@@ -9320,51 +9293,47 @@
       <c r="AH5" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="AI5" s="468">
-        <v>1</v>
-      </c>
+      <c r="AI5" s="468"/>
       <c r="AJ5" s="553"/>
       <c r="AK5" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="AL5" s="468">
-        <v>1</v>
-      </c>
+      <c r="AL5" s="468"/>
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="690" t="s">
+      <c r="A6" s="704" t="s">
         <v>285</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="661"/>
-      <c r="D6" s="662"/>
+      <c r="C6" s="629"/>
+      <c r="D6" s="630"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
-      <c r="G6" s="599"/>
-      <c r="I6" s="706"/>
+      <c r="G6" s="600"/>
+      <c r="I6" s="694"/>
       <c r="P6" s="61" t="s">
         <v>592</v>
       </c>
       <c r="R6" s="64">
         <f>R7-SUM(X2:X10)+R11</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S6" s="64">
         <f>S7+S11-SUM(V2:V10)</f>
         <v>3</v>
       </c>
-      <c r="AB6" s="709"/>
+      <c r="AB6" s="697"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF6" s="64">
         <f>AF7-SUM(AI2:AI10)+AF11</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AH6" s="6"/>
       <c r="AI6" s="525"/>
@@ -9372,7 +9341,7 @@
       <c r="AL6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="691"/>
+      <c r="A7" s="705"/>
       <c r="B7" s="100" t="s">
         <v>154</v>
       </c>
@@ -9382,8 +9351,8 @@
       <c r="D7" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="G7" s="599"/>
-      <c r="I7" s="706"/>
+      <c r="G7" s="600"/>
+      <c r="I7" s="694"/>
       <c r="M7" s="16" t="s">
         <v>347</v>
       </c>
@@ -9401,7 +9370,7 @@
       </c>
       <c r="R7" s="24">
         <f>3-R11</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S7" s="24">
         <f>3-S11</f>
@@ -9412,10 +9381,8 @@
       <c r="W7" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="X7" s="469">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="709"/>
+      <c r="X7" s="469"/>
+      <c r="AB7" s="697"/>
       <c r="AC7" s="99" t="s">
         <v>593</v>
       </c>
@@ -9424,28 +9391,24 @@
       </c>
       <c r="AE7" s="24">
         <f>8-AE11</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AF7" s="295">
         <f>8-AF11</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AH7" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AI7" s="469">
-        <v>2</v>
-      </c>
+      <c r="AI7" s="469"/>
       <c r="AJ7" s="553"/>
       <c r="AK7" s="6" t="s">
         <v>613</v>
       </c>
-      <c r="AL7" s="24">
-        <v>2</v>
-      </c>
+      <c r="AL7" s="24"/>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="692"/>
+      <c r="A8" s="706"/>
       <c r="B8" s="212" t="s">
         <v>28</v>
       </c>
@@ -9453,32 +9416,26 @@
       <c r="E8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="599"/>
-      <c r="I8" s="706"/>
+      <c r="G8" s="600"/>
+      <c r="I8" s="694"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6"/>
       <c r="V8" s="24"/>
       <c r="W8" s="6" t="s">
         <v>613</v>
       </c>
-      <c r="X8" s="470">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="709"/>
+      <c r="X8" s="470"/>
+      <c r="AB8" s="697"/>
       <c r="AC8" s="515"/>
       <c r="AH8" s="6" t="s">
         <v>612</v>
       </c>
-      <c r="AI8" s="470">
-        <v>1</v>
-      </c>
+      <c r="AI8" s="470"/>
       <c r="AJ8" s="553"/>
       <c r="AK8" s="6" t="s">
         <v>621</v>
       </c>
-      <c r="AL8" s="469">
-        <v>1</v>
-      </c>
+      <c r="AL8" s="469"/>
     </row>
     <row r="9" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="231" t="s">
@@ -9493,9 +9450,9 @@
       <c r="D9" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G9" s="599"/>
+      <c r="G9" s="600"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="706"/>
+      <c r="I9" s="694"/>
       <c r="M9" s="19" t="s">
         <v>525</v>
       </c>
@@ -9505,10 +9462,8 @@
       <c r="W9" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="X9" s="470">
-        <v>1</v>
-      </c>
-      <c r="AB9" s="709"/>
+      <c r="X9" s="470"/>
+      <c r="AB9" s="697"/>
       <c r="AC9" s="515"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9531,8 +9486,8 @@
         <f>Boat!W8</f>
         <v>39</v>
       </c>
-      <c r="G10" s="599"/>
-      <c r="I10" s="706"/>
+      <c r="G10" s="600"/>
+      <c r="I10" s="694"/>
       <c r="J10" s="24" t="s">
         <v>372</v>
       </c>
@@ -9547,29 +9502,25 @@
       <c r="V10" s="470"/>
       <c r="W10" s="6"/>
       <c r="X10" s="470"/>
-      <c r="AB10" s="709"/>
+      <c r="AB10" s="697"/>
       <c r="AC10" s="515"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
       <c r="AH10" s="6" t="s">
         <v>614</v>
       </c>
-      <c r="AI10" s="470">
-        <v>1</v>
-      </c>
+      <c r="AI10" s="470"/>
       <c r="AJ10" s="554"/>
       <c r="AK10" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="AL10" s="468">
-        <v>1</v>
-      </c>
+      <c r="AL10" s="468"/>
     </row>
     <row r="11" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="99" t="s">
         <v>183</v>
       </c>
-      <c r="B11" s="598" t="s">
+      <c r="B11" s="599" t="s">
         <v>382</v>
       </c>
       <c r="C11" s="171" t="s">
@@ -9578,8 +9529,8 @@
       <c r="D11" s="217" t="s">
         <v>265</v>
       </c>
-      <c r="G11" s="599"/>
-      <c r="I11" s="706"/>
+      <c r="G11" s="600"/>
+      <c r="I11" s="694"/>
       <c r="J11" s="24" t="s">
         <v>194</v>
       </c>
@@ -9600,18 +9551,18 @@
         <v>44</v>
       </c>
       <c r="R11" s="24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S11" s="24">
         <v>3</v>
       </c>
-      <c r="U11" s="711" t="s">
+      <c r="U11" s="699" t="s">
         <v>558</v>
       </c>
-      <c r="V11" s="712"/>
-      <c r="W11" s="712"/>
-      <c r="X11" s="713"/>
-      <c r="AB11" s="710"/>
+      <c r="V11" s="700"/>
+      <c r="W11" s="700"/>
+      <c r="X11" s="701"/>
+      <c r="AB11" s="698"/>
       <c r="AC11" s="99" t="s">
         <v>595</v>
       </c>
@@ -9619,30 +9570,30 @@
         <v>44</v>
       </c>
       <c r="AE11" s="24">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF11" s="24">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG11" s="414"/>
-      <c r="AH11" s="711" t="s">
+      <c r="AH11" s="699" t="s">
         <v>603</v>
       </c>
-      <c r="AI11" s="712"/>
-      <c r="AJ11" s="712"/>
-      <c r="AK11" s="712"/>
-      <c r="AL11" s="713"/>
+      <c r="AI11" s="700"/>
+      <c r="AJ11" s="700"/>
+      <c r="AK11" s="700"/>
+      <c r="AL11" s="701"/>
     </row>
     <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="227" t="s">
         <v>383</v>
       </c>
-      <c r="B12" s="600"/>
+      <c r="B12" s="601"/>
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="G12" s="599"/>
-      <c r="I12" s="706"/>
+      <c r="G12" s="600"/>
+      <c r="I12" s="694"/>
       <c r="J12" s="24" t="s">
         <v>516</v>
       </c>
@@ -9670,12 +9621,12 @@
       <c r="B13" s="216" t="s">
         <v>323</v>
       </c>
-      <c r="C13" s="598" t="s">
+      <c r="C13" s="599" t="s">
         <v>194</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="G13" s="599"/>
-      <c r="I13" s="706"/>
+      <c r="G13" s="600"/>
+      <c r="I13" s="694"/>
       <c r="J13" s="108" t="s">
         <v>548</v>
       </c>
@@ -9705,7 +9656,7 @@
       <c r="B14" s="173" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="600"/>
+      <c r="C14" s="601"/>
       <c r="D14" s="204" t="s">
         <v>153</v>
       </c>
@@ -9715,11 +9666,11 @@
       <c r="F14" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="G14" s="600"/>
+      <c r="G14" s="601"/>
       <c r="H14" s="206" t="s">
         <v>218</v>
       </c>
-      <c r="I14" s="706"/>
+      <c r="I14" s="694"/>
       <c r="U14" s="67" t="s">
         <v>80</v>
       </c>
@@ -9730,7 +9681,7 @@
       <c r="X14"/>
       <c r="Z14" s="68">
         <f>SUM(X23:X31)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9746,7 +9697,7 @@
       <c r="H15" s="271">
         <v>0</v>
       </c>
-      <c r="I15" s="706"/>
+      <c r="I15" s="694"/>
       <c r="J15" s="108" t="s">
         <v>153</v>
       </c>
@@ -9777,7 +9728,7 @@
       <c r="D16" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="I16" s="706"/>
+      <c r="I16" s="694"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9813,7 +9764,7 @@
       <c r="G17" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I17" s="706"/>
+      <c r="I17" s="694"/>
       <c r="L17" s="2" t="s">
         <v>426</v>
       </c>
@@ -9827,35 +9778,33 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="706"/>
+      <c r="I18" s="694"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="703" t="s">
+      <c r="O18" s="691" t="s">
         <v>517</v>
       </c>
-      <c r="P18" s="704"/>
+      <c r="P18" s="692"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
       <c r="R18" s="24">
         <f>5-R26</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S18" s="24">
         <f>5-S26</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U18" s="19"/>
       <c r="V18" s="24"/>
       <c r="W18" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="X18" s="24">
-        <v>1</v>
-      </c>
+      <c r="X18" s="24"/>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="706"/>
+      <c r="I19" s="694"/>
       <c r="M19" s="21" t="s">
         <v>425</v>
       </c>
@@ -9864,9 +9813,7 @@
       <c r="W19" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="X19" s="24">
-        <v>2</v>
-      </c>
+      <c r="X19" s="24"/>
     </row>
     <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="231" t="s">
@@ -9887,7 +9834,7 @@
       <c r="G20" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I20" s="706"/>
+      <c r="I20" s="694"/>
       <c r="K20" s="19" t="s">
         <v>422</v>
       </c>
@@ -9902,36 +9849,30 @@
       </c>
       <c r="R20" s="24">
         <f>R18-SUM(X16:X21)+R26</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S20" s="24">
         <f>S18-SUM(V16:V21)+S26</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U20" s="220" t="s">
         <v>87</v>
       </c>
-      <c r="V20" s="468">
-        <v>1</v>
-      </c>
+      <c r="V20" s="468"/>
       <c r="W20" s="6"/>
       <c r="X20" s="468"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="706"/>
+      <c r="I21" s="694"/>
       <c r="M21" s="216" t="s">
         <v>411</v>
       </c>
       <c r="U21" s="468"/>
-      <c r="V21" s="468">
-        <v>0</v>
-      </c>
+      <c r="V21" s="468"/>
       <c r="W21" s="19" t="s">
         <v>468</v>
       </c>
-      <c r="X21" s="468">
-        <v>1</v>
-      </c>
+      <c r="X21" s="468"/>
     </row>
     <row r="22" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="231" t="s">
@@ -9952,7 +9893,7 @@
       <c r="G22" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I22" s="706"/>
+      <c r="I22" s="694"/>
       <c r="P22" s="99" t="s">
         <v>591</v>
       </c>
@@ -9967,10 +9908,10 @@
       <c r="E23" s="283" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="706"/>
+      <c r="I23" s="694"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="U23" s="342"/>
       <c r="V23" s="183">
@@ -9984,16 +9925,16 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="706"/>
+      <c r="I24" s="694"/>
       <c r="U24" s="35"/>
       <c r="V24" s="509">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W24" s="54" t="s">
         <v>73</v>
       </c>
       <c r="X24" s="24">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10012,7 +9953,7 @@
       <c r="H25" s="191" t="s">
         <v>266</v>
       </c>
-      <c r="I25" s="706"/>
+      <c r="I25" s="694"/>
       <c r="J25" s="397" t="s">
         <v>269</v>
       </c>
@@ -10057,7 +9998,7 @@
       <c r="H26" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="I26" s="706"/>
+      <c r="I26" s="694"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10072,10 +10013,10 @@
         <v>44</v>
       </c>
       <c r="R26" s="24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S26" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T26" s="61" t="s">
         <v>556</v>
@@ -10092,7 +10033,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="706"/>
+      <c r="I27" s="694"/>
       <c r="O27" s="2" t="s">
         <v>98</v>
       </c>
@@ -10103,13 +10044,13 @@
       <c r="S27" s="112"/>
       <c r="U27" s="35"/>
       <c r="V27" s="509">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W27" s="54" t="s">
         <v>232</v>
       </c>
       <c r="X27" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10119,19 +10060,19 @@
       <c r="E28" s="215">
         <v>2</v>
       </c>
-      <c r="I28" s="706"/>
+      <c r="I28" s="694"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
       <c r="U28" s="35"/>
       <c r="V28" s="509">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W28" s="54" t="s">
         <v>87</v>
       </c>
       <c r="X28" s="24">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10141,7 +10082,7 @@
       <c r="H29" s="191" t="s">
         <v>267</v>
       </c>
-      <c r="I29" s="707"/>
+      <c r="I29" s="695"/>
       <c r="J29" s="324"/>
       <c r="L29" s="96" t="s">
         <v>273</v>
@@ -10188,24 +10129,17 @@
     <row r="31" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U31" s="480"/>
       <c r="V31" s="506">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W31" s="54" t="s">
         <v>468</v>
       </c>
       <c r="X31" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
-    <mergeCell ref="AH11:AL11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -10217,6 +10151,13 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
+    <mergeCell ref="AH11:AL11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10227,8 +10168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10328,14 +10269,14 @@
         <f ca="1">TODAY()</f>
         <v>45286</v>
       </c>
-      <c r="T1" s="742"/>
+      <c r="T1" s="736"/>
       <c r="U1" s="142"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="726" t="s">
+      <c r="X1" s="720" t="s">
         <v>441</v>
       </c>
-      <c r="Y1" s="727"/>
+      <c r="Y1" s="721"/>
       <c r="Z1" s="306">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10351,27 +10292,27 @@
       <c r="AD1" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="728" t="s">
+      <c r="AE1" s="722" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="729"/>
-      <c r="AG1" s="730"/>
-      <c r="AH1" s="731" t="s">
+      <c r="AF1" s="723"/>
+      <c r="AG1" s="724"/>
+      <c r="AH1" s="725" t="s">
         <v>293</v>
       </c>
-      <c r="AI1" s="732"/>
-      <c r="AJ1" s="733"/>
-      <c r="AK1" s="659" t="s">
+      <c r="AI1" s="726"/>
+      <c r="AJ1" s="727"/>
+      <c r="AK1" s="614" t="s">
         <v>616</v>
       </c>
       <c r="AL1" s="551" t="s">
         <v>617</v>
       </c>
-      <c r="AM1" s="723" t="s">
+      <c r="AM1" s="717" t="s">
         <v>444</v>
       </c>
-      <c r="AN1" s="724"/>
-      <c r="AO1" s="725"/>
+      <c r="AN1" s="718"/>
+      <c r="AO1" s="719"/>
       <c r="AR1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10384,29 +10325,29 @@
       </c>
       <c r="J2" s="318">
         <f>K2+L2</f>
-        <v>29</v>
-      </c>
-      <c r="K2" s="721">
+        <v>39</v>
+      </c>
+      <c r="K2" s="744">
         <f>SUM(K4:K37)</f>
         <v>6</v>
       </c>
-      <c r="L2" s="719">
+      <c r="L2" s="742">
         <f>SUM(L4:L37)</f>
-        <v>23</v>
-      </c>
-      <c r="M2" s="734">
+        <v>33</v>
+      </c>
+      <c r="M2" s="728">
         <f>SUM(M5:M30)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="736">
+      <c r="N2" s="730">
         <f>SUM(N4:N29)</f>
         <v>9</v>
       </c>
-      <c r="O2" s="738">
+      <c r="O2" s="732">
         <f>SUM(O4:O29)</f>
         <v>9</v>
       </c>
-      <c r="P2" s="666">
+      <c r="P2" s="638">
         <f>SUM(N30:N37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -10419,14 +10360,14 @@
       <c r="S2" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="T2" s="743"/>
+      <c r="T2" s="737"/>
       <c r="U2" s="537" t="s">
         <v>262</v>
       </c>
       <c r="V2" s="482" t="s">
         <v>219</v>
       </c>
-      <c r="W2" s="740" t="s">
+      <c r="W2" s="734" t="s">
         <v>234</v>
       </c>
       <c r="X2" s="483" t="s">
@@ -10468,7 +10409,7 @@
       <c r="AJ2" s="150" t="s">
         <v>288</v>
       </c>
-      <c r="AK2" s="660"/>
+      <c r="AK2" s="615"/>
       <c r="AL2" s="592" t="s">
         <v>288</v>
       </c>
@@ -10496,12 +10437,12 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="K3" s="722"/>
-      <c r="L3" s="720"/>
-      <c r="M3" s="735"/>
-      <c r="N3" s="737"/>
-      <c r="O3" s="739"/>
-      <c r="P3" s="667"/>
+      <c r="K3" s="745"/>
+      <c r="L3" s="743"/>
+      <c r="M3" s="729"/>
+      <c r="N3" s="731"/>
+      <c r="O3" s="733"/>
+      <c r="P3" s="639"/>
       <c r="Q3" s="172">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10509,7 +10450,7 @@
       <c r="S3" s="159" t="s">
         <v>244</v>
       </c>
-      <c r="T3" s="744"/>
+      <c r="T3" s="738"/>
       <c r="U3" s="538">
         <f>SUM(U4:U29)</f>
         <v>12</v>
@@ -10518,7 +10459,7 @@
         <f>SUM(V4:V29)</f>
         <v>39</v>
       </c>
-      <c r="W3" s="741"/>
+      <c r="W3" s="735"/>
       <c r="X3" s="485">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>8</v>
@@ -10624,7 +10565,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="716">
+      <c r="P4" s="739">
         <v>1</v>
       </c>
       <c r="Q4" s="20"/>
@@ -10710,7 +10651,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="717"/>
+      <c r="P5" s="740"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>340</v>
@@ -10804,7 +10745,7 @@
         <f>AC6</f>
         <v>0</v>
       </c>
-      <c r="P6" s="717"/>
+      <c r="P6" s="740"/>
       <c r="Q6" s="19" t="s">
         <v>335</v>
       </c>
@@ -10907,7 +10848,7 @@
         <f>AC7</f>
         <v>1</v>
       </c>
-      <c r="P7" s="717"/>
+      <c r="P7" s="740"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>335</v>
@@ -11012,7 +10953,9 @@
       <c r="K8" s="576">
         <v>1</v>
       </c>
-      <c r="L8" s="582"/>
+      <c r="L8" s="582">
+        <v>10</v>
+      </c>
       <c r="M8" s="107">
         <v>0</v>
       </c>
@@ -11023,7 +10966,7 @@
         <f t="shared" ref="O8:O37" si="10">AC8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="717"/>
+      <c r="P8" s="740"/>
       <c r="Q8" s="21" t="s">
         <v>233</v>
       </c>
@@ -11114,7 +11057,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="717"/>
+      <c r="P9" s="740"/>
       <c r="Q9" s="21" t="s">
         <v>335</v>
       </c>
@@ -11219,7 +11162,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="717"/>
+      <c r="P10" s="740"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>340</v>
@@ -11309,7 +11252,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="717"/>
+      <c r="P11" s="740"/>
       <c r="Q11" s="21" t="s">
         <v>335</v>
       </c>
@@ -11374,14 +11317,14 @@
       <c r="AR11" s="508"/>
     </row>
     <row r="12" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="626" t="s">
+      <c r="A12" s="676" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="681" t="s">
+      <c r="E12" s="626" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="262"/>
@@ -11406,7 +11349,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P12" s="717"/>
+      <c r="P12" s="740"/>
       <c r="Q12" s="21" t="s">
         <v>335</v>
       </c>
@@ -11483,14 +11426,14 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="628"/>
+      <c r="A13" s="678"/>
       <c r="B13" s="584">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="682"/>
+      <c r="E13" s="627"/>
       <c r="F13" s="172">
         <v>0</v>
       </c>
@@ -11514,7 +11457,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="717"/>
+      <c r="P13" s="740"/>
       <c r="Q13" s="21" t="s">
         <v>335</v>
       </c>
@@ -11596,7 +11539,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P14" s="717"/>
+      <c r="P14" s="740"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="200" t="s">
         <v>339</v>
@@ -11697,7 +11640,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P15" s="717"/>
+      <c r="P15" s="740"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="200" t="s">
         <v>339</v>
@@ -11789,7 +11732,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="717"/>
+      <c r="P16" s="740"/>
       <c r="Q16" s="21" t="s">
         <v>335</v>
       </c>
@@ -11890,7 +11833,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P17" s="717"/>
+      <c r="P17" s="740"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>341</v>
@@ -11990,7 +11933,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="717"/>
+      <c r="P18" s="740"/>
       <c r="Q18" s="21" t="s">
         <v>335</v>
       </c>
@@ -12080,7 +12023,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="717"/>
+      <c r="P19" s="740"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>334</v>
@@ -12188,11 +12131,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="718"/>
-      <c r="Q20" s="603" t="s">
+      <c r="P20" s="741"/>
+      <c r="Q20" s="604" t="s">
         <v>335</v>
       </c>
-      <c r="R20" s="683"/>
+      <c r="R20" s="628"/>
       <c r="S20" s="534" t="s">
         <v>85</v>
       </c>
@@ -12452,7 +12395,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="633" t="s">
+      <c r="E23" s="683" t="s">
         <v>289</v>
       </c>
       <c r="F23" s="180"/>
@@ -12557,7 +12500,7 @@
       <c r="C24" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E24" s="634"/>
+      <c r="E24" s="684"/>
       <c r="F24" s="172"/>
       <c r="H24" s="42"/>
       <c r="J24" s="571" t="s">
@@ -12579,10 +12522,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q24" s="603" t="s">
+      <c r="Q24" s="604" t="s">
         <v>335</v>
       </c>
-      <c r="R24" s="683"/>
+      <c r="R24" s="628"/>
       <c r="S24" s="534" t="s">
         <v>249</v>
       </c>
@@ -12861,7 +12804,7 @@
       <c r="AR26" s="508"/>
     </row>
     <row r="27" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="791"/>
+      <c r="B27" s="593"/>
       <c r="E27" s="31" t="s">
         <v>290</v>
       </c>
@@ -13238,8 +13181,8 @@
       <c r="AR31" s="508"/>
     </row>
     <row r="32" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="650"/>
-      <c r="B32" s="650"/>
+      <c r="A32" s="631"/>
+      <c r="B32" s="631"/>
       <c r="J32" s="572"/>
       <c r="K32" s="587"/>
       <c r="L32" s="581">
@@ -13711,7 +13654,7 @@
     </row>
     <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="21">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D37" s="382">
         <v>1</v>
@@ -13816,6 +13759,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13827,15 +13779,6 @@
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13900,10 +13843,10 @@
         <f ca="1">TODAY()</f>
         <v>45286</v>
       </c>
-      <c r="V1" s="603" t="s">
+      <c r="V1" s="604" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="683"/>
+      <c r="W1" s="628"/>
       <c r="X1" s="62" t="s">
         <v>101</v>
       </c>
@@ -13922,7 +13865,7 @@
       <c r="AC1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="759" t="s">
+      <c r="AD1" s="753" t="s">
         <v>211</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13939,10 +13882,10 @@
       <c r="E2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="790" t="s">
+      <c r="F2" s="752" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="747" t="s">
+      <c r="G2" s="780" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13970,10 +13913,10 @@
       <c r="U2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="726" t="s">
+      <c r="V2" s="720" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="727"/>
+      <c r="W2" s="721"/>
       <c r="X2" s="64" t="s">
         <v>109</v>
       </c>
@@ -13992,7 +13935,7 @@
       <c r="AC2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="760"/>
+      <c r="AD2" s="754"/>
       <c r="AE2" s="64" t="s">
         <v>98</v>
       </c>
@@ -14011,8 +13954,8 @@
       <c r="E3" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="630"/>
-      <c r="G3" s="748"/>
+      <c r="F3" s="680"/>
+      <c r="G3" s="781"/>
       <c r="H3" s="40" t="s">
         <v>80</v>
       </c>
@@ -14023,13 +13966,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="757" t="s">
+      <c r="O3" s="790" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="778" t="s">
+      <c r="P3" s="772" t="s">
         <v>217</v>
       </c>
-      <c r="Q3" s="779"/>
+      <c r="Q3" s="773"/>
       <c r="S3" s="57" t="s">
         <v>218</v>
       </c>
@@ -14039,15 +13982,15 @@
       <c r="W3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="AD3" s="760"/>
+      <c r="AD3" s="754"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="748"/>
+      <c r="G4" s="781"/>
       <c r="H4" s="6"/>
-      <c r="L4" s="687" t="s">
+      <c r="L4" s="688" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="758"/>
+      <c r="O4" s="791"/>
       <c r="T4" s="55" t="s">
         <v>97</v>
       </c>
@@ -14057,12 +14000,12 @@
       <c r="X4" s="67" t="s">
         <v>221</v>
       </c>
-      <c r="Y4" s="603" t="s">
+      <c r="Y4" s="604" t="s">
         <v>194</v>
       </c>
-      <c r="Z4" s="605"/>
-      <c r="AA4" s="683"/>
-      <c r="AD4" s="760"/>
+      <c r="Z4" s="606"/>
+      <c r="AA4" s="628"/>
+      <c r="AD4" s="754"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -14077,21 +14020,21 @@
       <c r="F5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="748"/>
+      <c r="G5" s="781"/>
       <c r="H5" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="765" t="s">
+      <c r="K5" s="759" t="s">
         <v>215</v>
       </c>
-      <c r="L5" s="780"/>
+      <c r="L5" s="774"/>
       <c r="M5" s="2" t="s">
         <v>213</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="O5" s="758"/>
+      <c r="O5" s="791"/>
       <c r="P5" s="108" t="s">
         <v>214</v>
       </c>
@@ -14107,11 +14050,11 @@
       <c r="U5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="768" t="s">
+      <c r="Y5" s="762" t="s">
         <v>282</v>
       </c>
-      <c r="Z5" s="769"/>
-      <c r="AD5" s="760"/>
+      <c r="Z5" s="763"/>
+      <c r="AD5" s="754"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -14121,16 +14064,16 @@
       <c r="E6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="748"/>
+      <c r="G6" s="781"/>
       <c r="H6" s="46" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="766"/>
-      <c r="L6" s="780"/>
-      <c r="O6" s="758"/>
+      <c r="K6" s="760"/>
+      <c r="L6" s="774"/>
+      <c r="O6" s="791"/>
       <c r="T6" s="2" t="s">
         <v>100</v>
       </c>
@@ -14140,23 +14083,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="760"/>
+      <c r="AD6" s="754"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="748"/>
+      <c r="G7" s="781"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="766"/>
-      <c r="L7" s="780"/>
+      <c r="K7" s="760"/>
+      <c r="L7" s="774"/>
       <c r="N7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="758"/>
+      <c r="O7" s="791"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="760"/>
+      <c r="AD7" s="754"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -14169,7 +14112,7 @@
       <c r="F8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="748"/>
+      <c r="G8" s="781"/>
       <c r="H8" s="50" t="s">
         <v>75</v>
       </c>
@@ -14179,41 +14122,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="766"/>
-      <c r="L8" s="780"/>
-      <c r="O8" s="758"/>
+      <c r="K8" s="760"/>
+      <c r="L8" s="774"/>
+      <c r="O8" s="791"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="762" t="s">
+      <c r="S8" s="756" t="s">
         <v>210</v>
       </c>
-      <c r="T8" s="763"/>
-      <c r="U8" s="763"/>
-      <c r="V8" s="763"/>
-      <c r="W8" s="763"/>
-      <c r="X8" s="763"/>
-      <c r="Y8" s="763"/>
-      <c r="Z8" s="763"/>
-      <c r="AA8" s="763"/>
-      <c r="AB8" s="763"/>
-      <c r="AC8" s="764"/>
-      <c r="AD8" s="760"/>
+      <c r="T8" s="757"/>
+      <c r="U8" s="757"/>
+      <c r="V8" s="757"/>
+      <c r="W8" s="757"/>
+      <c r="X8" s="757"/>
+      <c r="Y8" s="757"/>
+      <c r="Z8" s="757"/>
+      <c r="AA8" s="757"/>
+      <c r="AB8" s="757"/>
+      <c r="AC8" s="758"/>
+      <c r="AD8" s="754"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="784"/>
-      <c r="G9" s="748"/>
+      <c r="C9" s="746"/>
+      <c r="G9" s="781"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="766"/>
-      <c r="L9" s="751" t="s">
+      <c r="K9" s="760"/>
+      <c r="L9" s="784" t="s">
         <v>216</v>
       </c>
-      <c r="M9" s="752"/>
-      <c r="N9" s="753"/>
-      <c r="O9" s="758"/>
+      <c r="M9" s="785"/>
+      <c r="N9" s="786"/>
+      <c r="O9" s="791"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="760"/>
+      <c r="AD9" s="754"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="785"/>
+      <c r="C10" s="747"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>87</v>
@@ -14221,7 +14164,7 @@
       <c r="F10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="748"/>
+      <c r="G10" s="781"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>80</v>
@@ -14229,33 +14172,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="766"/>
-      <c r="M10" s="787" t="s">
+      <c r="K10" s="760"/>
+      <c r="M10" s="749" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="788"/>
-      <c r="O10" s="788"/>
-      <c r="P10" s="788"/>
-      <c r="Q10" s="788"/>
-      <c r="R10" s="788"/>
-      <c r="S10" s="788"/>
-      <c r="T10" s="788"/>
-      <c r="U10" s="788"/>
-      <c r="V10" s="788"/>
-      <c r="W10" s="788"/>
-      <c r="X10" s="788"/>
-      <c r="Y10" s="788"/>
-      <c r="Z10" s="788"/>
-      <c r="AA10" s="788"/>
-      <c r="AB10" s="788"/>
-      <c r="AC10" s="789"/>
-      <c r="AD10" s="760"/>
+      <c r="N10" s="750"/>
+      <c r="O10" s="750"/>
+      <c r="P10" s="750"/>
+      <c r="Q10" s="750"/>
+      <c r="R10" s="750"/>
+      <c r="S10" s="750"/>
+      <c r="T10" s="750"/>
+      <c r="U10" s="750"/>
+      <c r="V10" s="750"/>
+      <c r="W10" s="750"/>
+      <c r="X10" s="750"/>
+      <c r="Y10" s="750"/>
+      <c r="Z10" s="750"/>
+      <c r="AA10" s="750"/>
+      <c r="AB10" s="750"/>
+      <c r="AC10" s="751"/>
+      <c r="AD10" s="754"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="786"/>
-      <c r="G11" s="748"/>
+      <c r="C11" s="748"/>
+      <c r="G11" s="781"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="766"/>
+      <c r="K11" s="760"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14263,17 +14206,17 @@
       <c r="Y11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="776" t="s">
+      <c r="Z11" s="770" t="s">
         <v>120</v>
       </c>
-      <c r="AA11" s="777"/>
+      <c r="AA11" s="771"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="AD11" s="760"/>
+      <c r="AD11" s="754"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14286,7 +14229,7 @@
       <c r="F12" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="748"/>
+      <c r="G12" s="781"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>80</v>
@@ -14294,8 +14237,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="766"/>
-      <c r="L12" s="781" t="s">
+      <c r="K12" s="760"/>
+      <c r="L12" s="775" t="s">
         <v>92</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14310,7 +14253,7 @@
       <c r="Q12" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="598" t="s">
+      <c r="S12" s="599" t="s">
         <v>106</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -14326,26 +14269,26 @@
         <v>115</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="770" t="s">
+      <c r="AA12" s="764" t="s">
         <v>125</v>
       </c>
-      <c r="AB12" s="771"/>
+      <c r="AB12" s="765"/>
       <c r="AC12" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="AD12" s="760"/>
+      <c r="AD12" s="754"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="784"/>
-      <c r="G13" s="748"/>
-      <c r="K13" s="766"/>
-      <c r="L13" s="782"/>
+      <c r="C13" s="746"/>
+      <c r="G13" s="781"/>
+      <c r="K13" s="760"/>
+      <c r="L13" s="776"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="750" t="s">
+      <c r="Q13" s="783" t="s">
         <v>208</v>
       </c>
-      <c r="R13" s="639"/>
-      <c r="S13" s="599"/>
+      <c r="R13" s="645"/>
+      <c r="S13" s="600"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
         <v>131</v>
@@ -14353,17 +14296,17 @@
       <c r="X13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA13" s="772"/>
-      <c r="AB13" s="773"/>
-      <c r="AD13" s="760"/>
+      <c r="AA13" s="766"/>
+      <c r="AB13" s="767"/>
+      <c r="AD13" s="754"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C14" s="786"/>
+      <c r="C14" s="748"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="748"/>
+      <c r="G14" s="781"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14371,8 +14314,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="766"/>
-      <c r="L14" s="782"/>
+      <c r="K14" s="760"/>
+      <c r="L14" s="776"/>
       <c r="M14" s="21" t="s">
         <v>110</v>
       </c>
@@ -14382,7 +14325,7 @@
       <c r="R14" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="599"/>
+      <c r="S14" s="600"/>
       <c r="T14" s="77" t="s">
         <v>129</v>
       </c>
@@ -14393,9 +14336,9 @@
       <c r="Y14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="772"/>
-      <c r="AB14" s="773"/>
-      <c r="AD14" s="760"/>
+      <c r="AA14" s="766"/>
+      <c r="AB14" s="767"/>
+      <c r="AD14" s="754"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14410,20 +14353,20 @@
       <c r="F15" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="748"/>
+      <c r="G15" s="781"/>
       <c r="H15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="766"/>
-      <c r="L15" s="783"/>
-      <c r="Q15" s="750" t="s">
+      <c r="K15" s="760"/>
+      <c r="L15" s="777"/>
+      <c r="Q15" s="783" t="s">
         <v>209</v>
       </c>
-      <c r="R15" s="639"/>
-      <c r="S15" s="599"/>
+      <c r="R15" s="645"/>
+      <c r="S15" s="600"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
         <v>44</v>
@@ -14431,14 +14374,14 @@
       <c r="X15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AA15" s="772"/>
-      <c r="AB15" s="773"/>
-      <c r="AD15" s="760"/>
+      <c r="AA15" s="766"/>
+      <c r="AB15" s="767"/>
+      <c r="AD15" s="754"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="748"/>
-      <c r="K16" s="766"/>
+      <c r="G16" s="781"/>
+      <c r="K16" s="760"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>108</v>
@@ -14446,7 +14389,7 @@
       <c r="R16" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="S16" s="599"/>
+      <c r="S16" s="600"/>
       <c r="T16" s="76" t="s">
         <v>128</v>
       </c>
@@ -14457,34 +14400,34 @@
       <c r="Z16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AA16" s="772"/>
-      <c r="AB16" s="773"/>
-      <c r="AD16" s="760"/>
+      <c r="AA16" s="766"/>
+      <c r="AB16" s="767"/>
+      <c r="AD16" s="754"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="745" t="s">
+      <c r="F17" s="778" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="748"/>
+      <c r="G17" s="781"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="766"/>
-      <c r="S17" s="599"/>
+      <c r="K17" s="760"/>
+      <c r="S17" s="600"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA17" s="772"/>
-      <c r="AB17" s="773"/>
-      <c r="AD17" s="760"/>
+      <c r="AA17" s="766"/>
+      <c r="AB17" s="767"/>
+      <c r="AD17" s="754"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14494,58 +14437,61 @@
       <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="746"/>
-      <c r="G18" s="748"/>
+      <c r="F18" s="779"/>
+      <c r="G18" s="781"/>
       <c r="H18" s="108" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="766"/>
+      <c r="K18" s="760"/>
       <c r="O18" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="S18" s="599"/>
+      <c r="S18" s="600"/>
       <c r="U18" s="76" t="s">
         <v>132</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AA18" s="774"/>
-      <c r="AB18" s="775"/>
-      <c r="AD18" s="760"/>
+      <c r="AA18" s="768"/>
+      <c r="AB18" s="769"/>
+      <c r="AD18" s="754"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="G19" s="749"/>
-      <c r="K19" s="767"/>
+      <c r="G19" s="782"/>
+      <c r="K19" s="761"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="754" t="s">
+      <c r="R19" s="787" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="755"/>
-      <c r="T19" s="756"/>
+      <c r="S19" s="788"/>
+      <c r="T19" s="789"/>
       <c r="V19" s="77" t="s">
         <v>114</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AD19" s="761"/>
+      <c r="AD19" s="755"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14557,14 +14503,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>